<commit_message>
Fix new numbers in phone list
</commit_message>
<xml_diff>
--- a/report/Debug/report_sheet.xlsx
+++ b/report/Debug/report_sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7965" yWindow="-120" windowWidth="10815" windowHeight="7995" tabRatio="881" activeTab="12"/>
+    <workbookView xWindow="7965" yWindow="-120" windowWidth="10815" windowHeight="7995" tabRatio="881" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="CONTROLS" sheetId="4" r:id="rId1"/>
@@ -12869,8 +12869,8 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView view="pageBreakPreview" topLeftCell="B4" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14714,7 +14714,7 @@
       </c>
       <c r="I34" s="25">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D34,MATCH(I$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J34" s="31"/>
       <c r="K34" s="36">
@@ -14727,7 +14727,7 @@
       </c>
       <c r="M34" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D34,MATCH(M$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N34" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D34,MATCH(N$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -14735,15 +14735,15 @@
       </c>
       <c r="O34" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D34,MATCH(O$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P34" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D34,MATCH(P$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="Q34" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D34,MATCH(Q$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="R34" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D34,MATCH(R$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -14782,7 +14782,7 @@
       </c>
       <c r="I35" s="37">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J35" s="32"/>
       <c r="K35" s="37">
@@ -14795,7 +14795,7 @@
       </c>
       <c r="M35" s="37">
         <f t="shared" si="5"/>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N35" s="37">
         <f t="shared" si="5"/>
@@ -14803,15 +14803,15 @@
       </c>
       <c r="O35" s="37">
         <f t="shared" si="5"/>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P35" s="37">
         <f t="shared" si="5"/>
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="Q35" s="37">
         <f t="shared" si="5"/>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="R35" s="37">
         <f t="shared" si="5"/>
@@ -17434,7 +17434,7 @@
       </c>
       <c r="M38" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D38,MATCH(M$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N38" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D38,MATCH(N$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -17502,7 +17502,7 @@
       </c>
       <c r="M39" s="37">
         <f t="shared" si="7"/>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N39" s="37">
         <f t="shared" si="7"/>
@@ -18028,8 +18028,8 @@
   </sheetPr>
   <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B7" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+    <sheetView view="pageBreakPreview" topLeftCell="B7" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32949,7 +32949,7 @@
         <v>14</v>
       </c>
       <c r="N227" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O227" s="17">
         <v>5</v>
@@ -36302,22 +36302,22 @@
         <v>4</v>
       </c>
       <c r="J2" s="17">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K2" s="17">
         <v>9</v>
       </c>
       <c r="L2" s="17">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M2" s="17">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="N2" s="17">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="O2" s="17">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P2" s="17">
         <v>6</v>
@@ -36355,7 +36355,7 @@
         <v>3</v>
       </c>
       <c r="J3" s="17">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K3" s="17">
         <v>23</v>
@@ -36452,7 +36452,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="17">
         <v>0</v>
@@ -36473,7 +36473,7 @@
         <v>73</v>
       </c>
       <c r="N5" s="17">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O5" s="17">
         <v>28</v>
@@ -36611,7 +36611,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H8" s="17">
         <v>0</v>
@@ -36717,7 +36717,7 @@
         <v>31</v>
       </c>
       <c r="G10" s="17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H10" s="17">
         <v>3</v>
@@ -36726,19 +36726,19 @@
         <v>3</v>
       </c>
       <c r="J10" s="17">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K10" s="17">
         <v>17</v>
       </c>
       <c r="L10" s="17">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M10" s="17">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="N10" s="17">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O10" s="17">
         <v>35</v>
@@ -36823,7 +36823,7 @@
         <v>17</v>
       </c>
       <c r="G12" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H12" s="17">
         <v>2</v>
@@ -41007,7 +41007,7 @@
       </c>
       <c r="I62" s="25">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D62,MATCH(I$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J62" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D62,MATCH(J$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -41083,7 +41083,7 @@
       </c>
       <c r="I63" s="25">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D63,MATCH(I$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J63" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D63,MATCH(J$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -41247,7 +41247,7 @@
       </c>
       <c r="L65" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D65,MATCH(L$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M65" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D65,MATCH(M$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -41255,19 +41255,19 @@
       </c>
       <c r="N65" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D65,MATCH(N$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O65" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D65,MATCH(O$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="P65" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D65,MATCH(P$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="Q65" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D65,MATCH(Q$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="R65" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D65,MATCH(R$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -41311,7 +41311,7 @@
       </c>
       <c r="I66" s="25">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D66,MATCH(I$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J66" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D66,MATCH(J$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -41339,7 +41339,7 @@
       </c>
       <c r="P66" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D66,MATCH(P$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q66" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D66,MATCH(Q$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -41463,7 +41463,7 @@
       </c>
       <c r="I68" s="25">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D68,MATCH(I$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J68" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D68,MATCH(J$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -41475,7 +41475,7 @@
       </c>
       <c r="L68" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D68,MATCH(L$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M68" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D68,MATCH(M$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -41483,15 +41483,15 @@
       </c>
       <c r="N68" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D68,MATCH(N$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O68" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D68,MATCH(O$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="P68" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D68,MATCH(P$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q68" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D68,MATCH(Q$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -41551,7 +41551,7 @@
       </c>
       <c r="L69" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D69,MATCH(L$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M69" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D69,MATCH(M$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -41682,7 +41682,7 @@
       </c>
       <c r="I71" s="40">
         <f t="shared" ref="I71" si="51">SUM(I60:I70)</f>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J71" s="40">
         <f t="shared" ref="J71" si="52">SUM(J60:J70)</f>
@@ -41694,7 +41694,7 @@
       </c>
       <c r="L71" s="40">
         <f t="shared" ref="L71" si="54">SUM(L60:L70)</f>
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="M71" s="40">
         <f t="shared" ref="M71" si="55">SUM(M60:M70)</f>
@@ -41702,19 +41702,19 @@
       </c>
       <c r="N71" s="40">
         <f t="shared" ref="N71" si="56">SUM(N60:N70)</f>
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="O71" s="40">
         <f t="shared" ref="O71" si="57">SUM(O60:O70)</f>
-        <v>1112</v>
+        <v>1130</v>
       </c>
       <c r="P71" s="40">
         <f t="shared" ref="P71" si="58">SUM(P60:P70)</f>
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="Q71" s="40">
         <f t="shared" ref="Q71" si="59">SUM(Q60:Q70)</f>
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="R71" s="40">
         <f t="shared" ref="R71" si="60">SUM(R60:R70)</f>
@@ -41749,7 +41749,7 @@
       </c>
       <c r="I72" s="26">
         <f t="shared" si="62"/>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J72" s="26">
         <f t="shared" ref="J72" si="63">J71+J59+J47+J35+J23</f>
@@ -41761,7 +41761,7 @@
       </c>
       <c r="L72" s="26">
         <f t="shared" ref="L72" si="65">L71+L59+L47+L35+L23</f>
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="M72" s="26">
         <f t="shared" ref="M72" si="66">M71+M59+M47+M35+M23</f>
@@ -41769,19 +41769,19 @@
       </c>
       <c r="N72" s="26">
         <f t="shared" ref="N72" si="67">N71+N59+N47+N35+N23</f>
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="O72" s="26">
         <f t="shared" ref="O72" si="68">O71+O59+O47+O35+O23</f>
-        <v>1112</v>
+        <v>1130</v>
       </c>
       <c r="P72" s="26">
         <f t="shared" ref="P72" si="69">P71+P59+P47+P35+P23</f>
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="Q72" s="26">
         <f t="shared" ref="Q72" si="70">Q71+Q59+Q47+Q35+Q23</f>
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="R72" s="26">
         <f t="shared" ref="R72" si="71">R71+R59+R47+R35+R23</f>
@@ -46334,7 +46334,7 @@
       </c>
       <c r="I30" s="25">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D30,MATCH(I$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J30" s="31"/>
       <c r="K30" s="36">
@@ -46402,7 +46402,7 @@
       </c>
       <c r="I31" s="37">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J31" s="32"/>
       <c r="K31" s="37">
@@ -46780,7 +46780,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="B2" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48214,7 +48214,7 @@
       </c>
       <c r="I28" s="25">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D28,MATCH(I$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J28" s="31"/>
       <c r="K28" s="36">
@@ -48282,7 +48282,7 @@
       </c>
       <c r="I29" s="37">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J29" s="32"/>
       <c r="K29" s="37">
@@ -50904,8 +50904,8 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="W30" sqref="W30"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31:T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52590,7 +52590,7 @@
       </c>
       <c r="M31" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D31,MATCH(M$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N31" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D31,MATCH(N$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -52598,19 +52598,19 @@
       </c>
       <c r="O31" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D31,MATCH(O$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P31" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D31,MATCH(P$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="Q31" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D31,MATCH(Q$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="R31" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D31,MATCH(R$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="S31" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D31,MATCH(S$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -52658,7 +52658,7 @@
       </c>
       <c r="M32" s="37">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N32" s="37">
         <f t="shared" si="3"/>
@@ -52666,19 +52666,19 @@
       </c>
       <c r="O32" s="37">
         <f t="shared" si="3"/>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P32" s="37">
         <f t="shared" si="3"/>
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="Q32" s="37">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="R32" s="37">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="S32" s="37">
         <f t="shared" si="3"/>
@@ -53154,7 +53154,7 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53574,7 +53574,7 @@
       </c>
       <c r="Q12" s="25">
         <f>IFERROR(INDEX(REPORT_DATA_BY_COMP!$A:$AA,$D12,MATCH(Q$10,REPORT_DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" s="25">
         <f>IFERROR(INDEX(REPORT_DATA_BY_COMP!$A:$AA,$D12,MATCH(R$10,REPORT_DATA_BY_COMP!$A$1:$AA$1,0)), "")</f>
@@ -53801,7 +53801,7 @@
       </c>
       <c r="Q15" s="26">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R15" s="26">
         <f t="shared" si="1"/>
@@ -54589,7 +54589,7 @@
       </c>
       <c r="I28" s="25">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D28,MATCH(I$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J28" s="31"/>
       <c r="K28" s="36">
@@ -54618,7 +54618,7 @@
       </c>
       <c r="Q28" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D28,MATCH(Q$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R28" s="36">
         <f>IFERROR(INDEX(REPORT_DATA_BY_ZONE!$A:$Z,$D28,MATCH(R$10,REPORT_DATA_BY_ZONE!$A$1:$Z$1,0)), "")</f>
@@ -54657,7 +54657,7 @@
       </c>
       <c r="I29" s="37">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29" s="32"/>
       <c r="K29" s="37">
@@ -54686,7 +54686,7 @@
       </c>
       <c r="Q29" s="37">
         <f t="shared" si="12"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R29" s="37">
         <f t="shared" si="12"/>
@@ -54749,7 +54749,7 @@
       </c>
       <c r="Q31" s="17">
         <f t="shared" si="13"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R31" s="17">
         <f t="shared" si="13"/>

</xml_diff>

<commit_message>
Add basic English reporting framework
</commit_message>
<xml_diff>
--- a/report/Debug/report_sheet.xlsx
+++ b/report/Debug/report_sheet.xlsx
@@ -12613,17 +12613,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P1:P8"/>
+    <mergeCell ref="Q1:Q8"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="S1:S8"/>
+    <mergeCell ref="T1:T8"/>
     <mergeCell ref="O1:O8"/>
     <mergeCell ref="E1:I8"/>
     <mergeCell ref="K1:K8"/>
     <mergeCell ref="L1:L8"/>
     <mergeCell ref="M1:M8"/>
     <mergeCell ref="N1:N8"/>
-    <mergeCell ref="P1:P8"/>
-    <mergeCell ref="Q1:Q8"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="S1:S8"/>
-    <mergeCell ref="T1:T8"/>
   </mergeCells>
   <conditionalFormatting sqref="K12:L13 K23:L26">
     <cfRule type="cellIs" dxfId="335" priority="83" operator="lessThan">
@@ -14891,17 +14891,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P1:P8"/>
+    <mergeCell ref="Q1:Q8"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="S1:S8"/>
+    <mergeCell ref="T1:T8"/>
     <mergeCell ref="O1:O8"/>
     <mergeCell ref="E1:I8"/>
     <mergeCell ref="K1:K8"/>
     <mergeCell ref="L1:L8"/>
     <mergeCell ref="M1:M8"/>
     <mergeCell ref="N1:N8"/>
-    <mergeCell ref="P1:P8"/>
-    <mergeCell ref="Q1:Q8"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="S1:S8"/>
-    <mergeCell ref="T1:T8"/>
   </mergeCells>
   <conditionalFormatting sqref="K12:L12">
     <cfRule type="cellIs" dxfId="279" priority="97" operator="lessThan">
@@ -17598,17 +17598,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P1:P8"/>
+    <mergeCell ref="Q1:Q8"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="S1:S8"/>
+    <mergeCell ref="T1:T8"/>
     <mergeCell ref="O1:O8"/>
     <mergeCell ref="E1:I8"/>
     <mergeCell ref="K1:K8"/>
     <mergeCell ref="L1:L8"/>
     <mergeCell ref="M1:M8"/>
     <mergeCell ref="N1:N8"/>
-    <mergeCell ref="P1:P8"/>
-    <mergeCell ref="Q1:Q8"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="S1:S8"/>
-    <mergeCell ref="T1:T8"/>
   </mergeCells>
   <conditionalFormatting sqref="K12:L13">
     <cfRule type="cellIs" dxfId="181" priority="97" operator="lessThan">
@@ -20542,17 +20542,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P1:P8"/>
+    <mergeCell ref="Q1:Q8"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="S1:S8"/>
+    <mergeCell ref="T1:T8"/>
     <mergeCell ref="O1:O8"/>
     <mergeCell ref="E1:I8"/>
     <mergeCell ref="K1:K8"/>
     <mergeCell ref="L1:L8"/>
     <mergeCell ref="M1:M8"/>
     <mergeCell ref="N1:N8"/>
-    <mergeCell ref="P1:P8"/>
-    <mergeCell ref="Q1:Q8"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="S1:S8"/>
-    <mergeCell ref="T1:T8"/>
   </mergeCells>
   <conditionalFormatting sqref="K12:L13 K25:L28 K31:L32">
     <cfRule type="cellIs" dxfId="83" priority="125" operator="lessThan">
@@ -41794,11 +41794,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="O1:O8"/>
-    <mergeCell ref="P1:P8"/>
-    <mergeCell ref="Q1:Q8"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="S1:S8"/>
     <mergeCell ref="M1:M8"/>
     <mergeCell ref="N1:N8"/>
     <mergeCell ref="B3:B5"/>
@@ -41806,6 +41801,11 @@
     <mergeCell ref="J1:J8"/>
     <mergeCell ref="K1:K8"/>
     <mergeCell ref="L1:L8"/>
+    <mergeCell ref="O1:O8"/>
+    <mergeCell ref="P1:P8"/>
+    <mergeCell ref="Q1:Q8"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="S1:S8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -42890,17 +42890,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P1:P8"/>
+    <mergeCell ref="Q1:Q8"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="S1:S8"/>
+    <mergeCell ref="T1:T8"/>
     <mergeCell ref="O1:O8"/>
     <mergeCell ref="E1:I8"/>
     <mergeCell ref="K1:K8"/>
     <mergeCell ref="L1:L8"/>
     <mergeCell ref="M1:M8"/>
     <mergeCell ref="N1:N8"/>
-    <mergeCell ref="P1:P8"/>
-    <mergeCell ref="Q1:Q8"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="S1:S8"/>
-    <mergeCell ref="T1:T8"/>
   </mergeCells>
   <conditionalFormatting sqref="K12:L13">
     <cfRule type="cellIs" dxfId="737" priority="39" operator="lessThan">
@@ -44559,17 +44559,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P1:P8"/>
+    <mergeCell ref="Q1:Q8"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="S1:S8"/>
+    <mergeCell ref="T1:T8"/>
     <mergeCell ref="O1:O8"/>
     <mergeCell ref="E1:I8"/>
     <mergeCell ref="K1:K8"/>
     <mergeCell ref="L1:L8"/>
     <mergeCell ref="M1:M8"/>
     <mergeCell ref="N1:N8"/>
-    <mergeCell ref="P1:P8"/>
-    <mergeCell ref="Q1:Q8"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="S1:S8"/>
-    <mergeCell ref="T1:T8"/>
   </mergeCells>
   <conditionalFormatting sqref="K12:L14">
     <cfRule type="cellIs" dxfId="710" priority="53" operator="lessThan">
@@ -46528,17 +46528,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P1:P8"/>
+    <mergeCell ref="Q1:Q8"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="S1:S8"/>
+    <mergeCell ref="T1:T8"/>
     <mergeCell ref="O1:O8"/>
     <mergeCell ref="E1:I8"/>
     <mergeCell ref="K1:K8"/>
     <mergeCell ref="L1:L8"/>
     <mergeCell ref="M1:M8"/>
     <mergeCell ref="N1:N8"/>
-    <mergeCell ref="P1:P8"/>
-    <mergeCell ref="Q1:Q8"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="S1:S8"/>
-    <mergeCell ref="T1:T8"/>
   </mergeCells>
   <conditionalFormatting sqref="K16:L18">
     <cfRule type="cellIs" dxfId="656" priority="54" operator="lessThan">
@@ -48391,17 +48391,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P1:P8"/>
+    <mergeCell ref="Q1:Q8"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="S1:S8"/>
+    <mergeCell ref="T1:T8"/>
     <mergeCell ref="O1:O8"/>
     <mergeCell ref="E1:I8"/>
     <mergeCell ref="K1:K8"/>
     <mergeCell ref="L1:L8"/>
     <mergeCell ref="M1:M8"/>
     <mergeCell ref="N1:N8"/>
-    <mergeCell ref="P1:P8"/>
-    <mergeCell ref="Q1:Q8"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="S1:S8"/>
-    <mergeCell ref="T1:T8"/>
   </mergeCells>
   <conditionalFormatting sqref="K12:L13">
     <cfRule type="cellIs" dxfId="601" priority="55" operator="lessThan">
@@ -50590,17 +50590,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P1:P8"/>
+    <mergeCell ref="Q1:Q8"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="S1:S8"/>
+    <mergeCell ref="T1:T8"/>
     <mergeCell ref="O1:O8"/>
     <mergeCell ref="E1:I8"/>
     <mergeCell ref="K1:K8"/>
     <mergeCell ref="L1:L8"/>
     <mergeCell ref="M1:M8"/>
     <mergeCell ref="N1:N8"/>
-    <mergeCell ref="P1:P8"/>
-    <mergeCell ref="Q1:Q8"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="S1:S8"/>
-    <mergeCell ref="T1:T8"/>
   </mergeCells>
   <conditionalFormatting sqref="K12:L13">
     <cfRule type="cellIs" dxfId="545" priority="69" operator="lessThan">
@@ -50905,7 +50905,7 @@
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:T31"/>
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52781,17 +52781,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="E1:I8"/>
-    <mergeCell ref="K1:K8"/>
-    <mergeCell ref="L1:L8"/>
-    <mergeCell ref="M1:M8"/>
-    <mergeCell ref="N1:N8"/>
     <mergeCell ref="T1:T8"/>
     <mergeCell ref="O1:O8"/>
     <mergeCell ref="P1:P8"/>
     <mergeCell ref="Q1:Q8"/>
     <mergeCell ref="R1:R8"/>
     <mergeCell ref="S1:S8"/>
+    <mergeCell ref="E1:I8"/>
+    <mergeCell ref="K1:K8"/>
+    <mergeCell ref="L1:L8"/>
+    <mergeCell ref="M1:M8"/>
+    <mergeCell ref="N1:N8"/>
   </mergeCells>
   <conditionalFormatting sqref="K12:L13">
     <cfRule type="cellIs" dxfId="475" priority="97" operator="lessThan">
@@ -54778,17 +54778,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P1:P8"/>
+    <mergeCell ref="Q1:Q8"/>
+    <mergeCell ref="R1:R8"/>
+    <mergeCell ref="S1:S8"/>
+    <mergeCell ref="T1:T8"/>
     <mergeCell ref="O1:O8"/>
     <mergeCell ref="E1:I8"/>
     <mergeCell ref="K1:K8"/>
     <mergeCell ref="L1:L8"/>
     <mergeCell ref="M1:M8"/>
     <mergeCell ref="N1:N8"/>
-    <mergeCell ref="P1:P8"/>
-    <mergeCell ref="Q1:Q8"/>
-    <mergeCell ref="R1:R8"/>
-    <mergeCell ref="S1:S8"/>
-    <mergeCell ref="T1:T8"/>
   </mergeCells>
   <conditionalFormatting sqref="K12:L12">
     <cfRule type="cellIs" dxfId="391" priority="55" operator="lessThan">

</xml_diff>